<commit_message>
not sure how I fixed connect.php but I did
</commit_message>
<xml_diff>
--- a/db/Mock Database.xlsx
+++ b/db/Mock Database.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avrsnsMac/dropship-iphonecase/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/AnimeCase/dropship-iphonecase/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="440" windowWidth="25520" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="6760" windowWidth="25520" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -440,7 +440,7 @@
   <dimension ref="B2:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>